<commit_message>
Reworked logic of adding actions. All works.
</commit_message>
<xml_diff>
--- a/public/Data/1_4_2020.xlsx
+++ b/public/Data/1_4_2020.xlsx
@@ -11,27 +11,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
   <si>
     <t>No</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Action</t>
-  </si>
-  <si>
-    <t>Room</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>1</t>
+    <t>Ім'я</t>
+  </si>
+  <si>
+    <t>Дія</t>
+  </si>
+  <si>
+    <t>Аудиторія</t>
+  </si>
+  <si>
+    <t>Час</t>
+  </si>
+  <si>
+    <t>Статус</t>
+  </si>
+  <si>
+    <t>Софія</t>
+  </si>
+  <si>
+    <t>Ввійшов і Взяв ключ</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>Юрій</t>
+  </si>
+  <si>
+    <t>Ввійшов</t>
+  </si>
+  <si>
+    <t>Залишив ключ</t>
+  </si>
+  <si>
+    <t>Вийшов</t>
+  </si>
+  <si>
+    <t>out</t>
   </si>
 </sst>
 </file>
@@ -67,8 +88,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,7 +430,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F8"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
@@ -438,27 +460,147 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>100</v>
+      </c>
+      <c r="E2" s="1">
+        <v>43952.7268072338</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>43952.72700042824</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>100</v>
+      </c>
+      <c r="E4" s="1">
+        <v>43952.72717405093</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>100</v>
+      </c>
+      <c r="E5" s="1">
+        <v>43952.72725534722</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6">
+        <v>100</v>
+      </c>
+      <c r="E6" s="1">
+        <v>43952.72731216435</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>43952.72787479167</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>43952.72791855324</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
</xml_diff>